<commit_message>
Adds updated Status Tracker for Week 8
</commit_message>
<xml_diff>
--- a/Documents/StatusTracker.xlsx
+++ b/Documents/StatusTracker.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>PROJECT NUMBER</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Build bare bones website to practice new technology</t>
   </si>
   <si>
-    <t>Ongoing</t>
-  </si>
-  <si>
     <t>Week 3 (August 22 – August 28)</t>
   </si>
   <si>
@@ -184,7 +181,22 @@
     <t>Train the bot on all possible FAQs</t>
   </si>
   <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
     <t>Week 8 (Sep 27 - October 3)</t>
+  </si>
+  <si>
+    <t>Test Plan Writeup</t>
+  </si>
+  <si>
+    <t>Design Document Writeup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slides for R1 Presentation </t>
+  </si>
+  <si>
+    <t>Week 9 (October 4 - October 10)</t>
   </si>
 </sst>
 </file>
@@ -309,7 +321,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -341,6 +353,12 @@
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1427,7 +1445,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z1009"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2303,18 +2321,20 @@
       <c r="D21" s="5">
         <v>6</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="5">
+        <v>5.5</v>
+      </c>
       <c r="F21" t="s" s="10">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="6">
         <f>D21-E21</f>
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="I21" s="6">
         <f>H21/D21*100</f>
-        <v>100</v>
+        <v>8.333333333333332</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -2382,7 +2402,7 @@
     </row>
     <row r="23" ht="13.75" customHeight="1">
       <c r="A23" t="s" s="7">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2458,7 +2478,7 @@
     </row>
     <row r="25" ht="13.75" customHeight="1">
       <c r="A25" t="s" s="10">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s" s="10">
         <v>29</v>
@@ -2504,7 +2524,7 @@
     </row>
     <row r="26" ht="13.75" customHeight="1">
       <c r="A26" t="s" s="10">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s" s="10">
         <v>21</v>
@@ -2550,7 +2570,7 @@
     </row>
     <row r="27" ht="13.75" customHeight="1">
       <c r="A27" t="s" s="10">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s" s="10">
         <v>21</v>
@@ -2596,7 +2616,7 @@
     </row>
     <row r="28" ht="13.75" customHeight="1">
       <c r="A28" t="s" s="7">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -2764,7 +2784,7 @@
     </row>
     <row r="32" ht="13.75" customHeight="1">
       <c r="A32" t="s" s="10">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s" s="10">
         <v>21</v>
@@ -2810,7 +2830,7 @@
     </row>
     <row r="33" ht="13.75" customHeight="1">
       <c r="A33" t="s" s="10">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s" s="10">
         <v>21</v>
@@ -2856,7 +2876,7 @@
     </row>
     <row r="34" ht="13.75" customHeight="1">
       <c r="A34" t="s" s="7">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -2932,7 +2952,7 @@
     </row>
     <row r="36" ht="13.75" customHeight="1">
       <c r="A36" t="s" s="10">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s" s="10">
         <v>29</v>
@@ -2978,7 +2998,7 @@
     </row>
     <row r="37" ht="13.75" customHeight="1">
       <c r="A37" t="s" s="10">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s" s="10">
         <v>21</v>
@@ -2989,18 +3009,20 @@
       <c r="D37" s="5">
         <v>10</v>
       </c>
-      <c r="E37" s="5"/>
+      <c r="E37" s="5">
+        <v>9.5</v>
+      </c>
       <c r="F37" t="s" s="10">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="6">
         <f>D37-E37</f>
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="I37" s="6">
         <f>H37/D37*100</f>
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
@@ -3022,7 +3044,7 @@
     </row>
     <row r="38" ht="13.75" customHeight="1">
       <c r="A38" t="s" s="7">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -3098,7 +3120,7 @@
     </row>
     <row r="40" ht="13.75" customHeight="1">
       <c r="A40" t="s" s="10">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s" s="10">
         <v>21</v>
@@ -3109,18 +3131,20 @@
       <c r="D40" s="5">
         <v>2</v>
       </c>
-      <c r="E40" s="5"/>
+      <c r="E40" s="5">
+        <v>1.5</v>
+      </c>
       <c r="F40" t="s" s="10">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G40" s="5"/>
       <c r="H40" s="6">
         <f>D40-E40</f>
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I40" s="6">
         <f>H40/D40*100</f>
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
@@ -3142,7 +3166,7 @@
     </row>
     <row r="41" ht="13.75" customHeight="1">
       <c r="A41" t="s" s="7">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -3310,7 +3334,7 @@
     </row>
     <row r="45" ht="13.75" customHeight="1">
       <c r="A45" t="s" s="10">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s" s="10">
         <v>21</v>
@@ -3356,29 +3380,31 @@
     </row>
     <row r="46" ht="13.75" customHeight="1">
       <c r="A46" t="s" s="10">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s" s="10">
         <v>21</v>
       </c>
       <c r="C46" t="s" s="10">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D46" s="5">
         <v>3</v>
       </c>
-      <c r="E46" s="5"/>
+      <c r="E46" s="5">
+        <v>4</v>
+      </c>
       <c r="F46" t="s" s="10">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G46" s="5"/>
       <c r="H46" s="6">
         <f>D46-E46</f>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="I46" s="6">
         <f>H46/D46*100</f>
-        <v>100</v>
+        <v>-33.33333333333333</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="5"/>
@@ -3400,20 +3426,20 @@
     </row>
     <row r="47" ht="13.75" customHeight="1">
       <c r="A47" t="s" s="10">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" t="s" s="10">
         <v>21</v>
       </c>
       <c r="C47" t="s" s="10">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D47" s="5">
         <v>15</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" t="s" s="10">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="G47" s="5"/>
       <c r="H47" s="6">
@@ -3473,15 +3499,33 @@
       <c r="Z48" s="5"/>
     </row>
     <row r="49" ht="13.75" customHeight="1">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="A49" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="B49" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C49" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="D49" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E49" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F49" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G49" s="5"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
+      <c r="H49" s="6">
+        <f>D49-E49</f>
+        <v>0</v>
+      </c>
+      <c r="I49" s="6">
+        <f>H49/D49*100</f>
+        <v>0</v>
+      </c>
       <c r="J49" s="5"/>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
@@ -3501,15 +3545,33 @@
       <c r="Z49" s="5"/>
     </row>
     <row r="50" ht="13.75" customHeight="1">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
+      <c r="A50" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="B50" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="C50" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="D50" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="F50" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G50" s="5"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
+      <c r="H50" s="6">
+        <f>D50-E50</f>
+        <v>0.09999999999999998</v>
+      </c>
+      <c r="I50" s="6">
+        <f>H50/D50*100</f>
+        <v>20</v>
+      </c>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
@@ -3529,15 +3591,33 @@
       <c r="Z50" s="5"/>
     </row>
     <row r="51" ht="13.75" customHeight="1">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
+      <c r="A51" t="s" s="10">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C51" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="D51" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F51" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G51" s="5"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
+      <c r="H51" s="6">
+        <f>D51-E51</f>
+        <v>0.25</v>
+      </c>
+      <c r="I51" s="6">
+        <f>H51/D51*100</f>
+        <v>33.33333333333333</v>
+      </c>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
@@ -3557,15 +3637,33 @@
       <c r="Z51" s="5"/>
     </row>
     <row r="52" ht="13.75" customHeight="1">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
+      <c r="A52" t="s" s="10">
+        <v>58</v>
+      </c>
+      <c r="B52" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C52" t="s" s="10">
+        <v>24</v>
+      </c>
+      <c r="D52" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F52" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G52" s="5"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
+      <c r="H52" s="6">
+        <f>D52-E52</f>
+        <v>0.25</v>
+      </c>
+      <c r="I52" s="6">
+        <f>H52/D52*100</f>
+        <v>33.33333333333333</v>
+      </c>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
@@ -3585,15 +3683,33 @@
       <c r="Z52" s="5"/>
     </row>
     <row r="53" ht="13.75" customHeight="1">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
+      <c r="A53" t="s" s="10">
+        <v>59</v>
+      </c>
+      <c r="B53" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C53" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E53" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="F53" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G53" s="5"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
+      <c r="H53" s="6">
+        <f>D53-E53</f>
+        <v>-0.3</v>
+      </c>
+      <c r="I53" s="6">
+        <f>H53/D53*100</f>
+        <v>-60.00000000000001</v>
+      </c>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
@@ -3613,15 +3729,33 @@
       <c r="Z53" s="5"/>
     </row>
     <row r="54" ht="13.75" customHeight="1">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
+      <c r="A54" t="s" s="10">
+        <v>60</v>
+      </c>
+      <c r="B54" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C54" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="D54" s="5">
+        <v>2</v>
+      </c>
+      <c r="E54" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="F54" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G54" s="5"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
+      <c r="H54" s="6">
+        <f>D54-E54</f>
+        <v>-0.5</v>
+      </c>
+      <c r="I54" s="6">
+        <f>H54/D54*100</f>
+        <v>-25</v>
+      </c>
       <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
@@ -3641,13 +3775,15 @@
       <c r="Z54" s="5"/>
     </row>
     <row r="55" ht="13.75" customHeight="1">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
+      <c r="A55" t="s" s="7">
+        <v>61</v>
+      </c>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="J55" s="5"/>
@@ -3669,15 +3805,15 @@
       <c r="Z55" s="5"/>
     </row>
     <row r="56" ht="13.75" customHeight="1">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
       <c r="G56" s="5"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
@@ -30296,6 +30432,90 @@
       <c r="Y1006" s="5"/>
       <c r="Z1006" s="5"/>
     </row>
+    <row r="1007" ht="13.75" customHeight="1">
+      <c r="A1007" s="5"/>
+      <c r="B1007" s="5"/>
+      <c r="C1007" s="5"/>
+      <c r="D1007" s="5"/>
+      <c r="E1007" s="5"/>
+      <c r="F1007" s="5"/>
+      <c r="G1007" s="5"/>
+      <c r="H1007" s="6"/>
+      <c r="I1007" s="6"/>
+      <c r="J1007" s="5"/>
+      <c r="K1007" s="5"/>
+      <c r="L1007" s="5"/>
+      <c r="M1007" s="5"/>
+      <c r="N1007" s="5"/>
+      <c r="O1007" s="5"/>
+      <c r="P1007" s="5"/>
+      <c r="Q1007" s="5"/>
+      <c r="R1007" s="5"/>
+      <c r="S1007" s="5"/>
+      <c r="T1007" s="5"/>
+      <c r="U1007" s="5"/>
+      <c r="V1007" s="5"/>
+      <c r="W1007" s="5"/>
+      <c r="X1007" s="5"/>
+      <c r="Y1007" s="5"/>
+      <c r="Z1007" s="5"/>
+    </row>
+    <row r="1008" ht="13.75" customHeight="1">
+      <c r="A1008" s="5"/>
+      <c r="B1008" s="5"/>
+      <c r="C1008" s="5"/>
+      <c r="D1008" s="5"/>
+      <c r="E1008" s="5"/>
+      <c r="F1008" s="5"/>
+      <c r="G1008" s="5"/>
+      <c r="H1008" s="6"/>
+      <c r="I1008" s="6"/>
+      <c r="J1008" s="5"/>
+      <c r="K1008" s="5"/>
+      <c r="L1008" s="5"/>
+      <c r="M1008" s="5"/>
+      <c r="N1008" s="5"/>
+      <c r="O1008" s="5"/>
+      <c r="P1008" s="5"/>
+      <c r="Q1008" s="5"/>
+      <c r="R1008" s="5"/>
+      <c r="S1008" s="5"/>
+      <c r="T1008" s="5"/>
+      <c r="U1008" s="5"/>
+      <c r="V1008" s="5"/>
+      <c r="W1008" s="5"/>
+      <c r="X1008" s="5"/>
+      <c r="Y1008" s="5"/>
+      <c r="Z1008" s="5"/>
+    </row>
+    <row r="1009" ht="13.75" customHeight="1">
+      <c r="A1009" s="5"/>
+      <c r="B1009" s="5"/>
+      <c r="C1009" s="5"/>
+      <c r="D1009" s="5"/>
+      <c r="E1009" s="5"/>
+      <c r="F1009" s="5"/>
+      <c r="G1009" s="5"/>
+      <c r="H1009" s="6"/>
+      <c r="I1009" s="6"/>
+      <c r="J1009" s="5"/>
+      <c r="K1009" s="5"/>
+      <c r="L1009" s="5"/>
+      <c r="M1009" s="5"/>
+      <c r="N1009" s="5"/>
+      <c r="O1009" s="5"/>
+      <c r="P1009" s="5"/>
+      <c r="Q1009" s="5"/>
+      <c r="R1009" s="5"/>
+      <c r="S1009" s="5"/>
+      <c r="T1009" s="5"/>
+      <c r="U1009" s="5"/>
+      <c r="V1009" s="5"/>
+      <c r="W1009" s="5"/>
+      <c r="X1009" s="5"/>
+      <c r="Y1009" s="5"/>
+      <c r="Z1009" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
Adds updated Status Tracker up to Week 12
</commit_message>
<xml_diff>
--- a/Documents/StatusTracker.xlsx
+++ b/Documents/StatusTracker.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>PROJECT NUMBER</t>
   </si>
@@ -175,10 +175,13 @@
     <t>Go through Pandora Bots Tutorial</t>
   </si>
   <si>
-    <t>Anubhab Sen, Vighnesh Chenthil Kumar, Ananya Trivedi</t>
+    <t>Vighnesh Chenthil Kumar, Anubhab Sen</t>
   </si>
   <si>
     <t>Train the bot on all possible FAQs</t>
+  </si>
+  <si>
+    <t>Anubhab Sen, Vighnesh Chenthil Kumar, Ananya Trivedi</t>
   </si>
   <si>
     <t>Ongoing</t>
@@ -197,6 +200,24 @@
   </si>
   <si>
     <t>Week 9 (October 4 - October 10)</t>
+  </si>
+  <si>
+    <t>Week 10 (October 11 - October 17)</t>
+  </si>
+  <si>
+    <t>Week 11 (October 18 - October 24)</t>
+  </si>
+  <si>
+    <t>Research on shortlisted Food Startups</t>
+  </si>
+  <si>
+    <t>Week 12 (October 25 - October 31)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prepare FAQs for FitMeals </t>
+  </si>
+  <si>
+    <t>Train the bot with the FAQs for FitMeals</t>
   </si>
 </sst>
 </file>
@@ -321,7 +342,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -353,12 +374,6 @@
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1445,7 +1460,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z1009"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -3432,14 +3447,14 @@
         <v>21</v>
       </c>
       <c r="C47" t="s" s="10">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D47" s="5">
         <v>15</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" t="s" s="10">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G47" s="5"/>
       <c r="H47" s="6">
@@ -3470,7 +3485,7 @@
     </row>
     <row r="48" ht="13.75" customHeight="1">
       <c r="A48" t="s" s="7">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
@@ -3638,7 +3653,7 @@
     </row>
     <row r="52" ht="13.75" customHeight="1">
       <c r="A52" t="s" s="10">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s" s="10">
         <v>29</v>
@@ -3684,7 +3699,7 @@
     </row>
     <row r="53" ht="13.75" customHeight="1">
       <c r="A53" t="s" s="10">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B53" t="s" s="10">
         <v>29</v>
@@ -3730,7 +3745,7 @@
     </row>
     <row r="54" ht="13.75" customHeight="1">
       <c r="A54" t="s" s="10">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B54" t="s" s="10">
         <v>29</v>
@@ -3776,7 +3791,7 @@
     </row>
     <row r="55" ht="13.75" customHeight="1">
       <c r="A55" t="s" s="7">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -3805,15 +3820,33 @@
       <c r="Z55" s="5"/>
     </row>
     <row r="56" ht="13.75" customHeight="1">
-      <c r="A56" s="11"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
+      <c r="A56" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="B56" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C56" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="D56" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E56" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F56" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G56" s="5"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
+      <c r="H56" s="6">
+        <f>D56-E56</f>
+        <v>0</v>
+      </c>
+      <c r="I56" s="6">
+        <f>H56/D56*100</f>
+        <v>0</v>
+      </c>
       <c r="J56" s="5"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
@@ -3833,13 +3866,15 @@
       <c r="Z56" s="5"/>
     </row>
     <row r="57" ht="13.75" customHeight="1">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
+      <c r="A57" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
       <c r="J57" s="5"/>
@@ -3861,15 +3896,33 @@
       <c r="Z57" s="5"/>
     </row>
     <row r="58" ht="13.75" customHeight="1">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
+      <c r="A58" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="B58" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C58" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="D58" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E58" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F58" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G58" s="5"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
+      <c r="H58" s="6">
+        <f>D58-E58</f>
+        <v>0</v>
+      </c>
+      <c r="I58" s="6">
+        <f>H58/D58*100</f>
+        <v>0</v>
+      </c>
       <c r="J58" s="5"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
@@ -3889,13 +3942,15 @@
       <c r="Z58" s="5"/>
     </row>
     <row r="59" ht="13.75" customHeight="1">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
+      <c r="A59" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
       <c r="J59" s="5"/>
@@ -3917,15 +3972,33 @@
       <c r="Z59" s="5"/>
     </row>
     <row r="60" ht="13.75" customHeight="1">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
+      <c r="A60" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="B60" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C60" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="D60" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E60" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F60" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G60" s="5"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
+      <c r="H60" s="6">
+        <f>D60-E60</f>
+        <v>0</v>
+      </c>
+      <c r="I60" s="6">
+        <f>H60/D60*100</f>
+        <v>0</v>
+      </c>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
@@ -3945,15 +4018,33 @@
       <c r="Z60" s="5"/>
     </row>
     <row r="61" ht="13.75" customHeight="1">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
+      <c r="A61" t="s" s="10">
+        <v>65</v>
+      </c>
+      <c r="B61" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="C61" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="D61" s="5">
+        <v>1</v>
+      </c>
+      <c r="E61" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F61" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G61" s="5"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
+      <c r="H61" s="6">
+        <f>D61-E61</f>
+        <v>0.5</v>
+      </c>
+      <c r="I61" s="6">
+        <f>H61/D61*100</f>
+        <v>50</v>
+      </c>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
@@ -3973,13 +4064,15 @@
       <c r="Z61" s="5"/>
     </row>
     <row r="62" ht="13.75" customHeight="1">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
+      <c r="A62" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
       <c r="J62" s="5"/>
@@ -4001,15 +4094,33 @@
       <c r="Z62" s="5"/>
     </row>
     <row r="63" ht="13.75" customHeight="1">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
+      <c r="A63" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="B63" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="D63" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E63" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F63" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G63" s="5"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="6"/>
+      <c r="H63" s="6">
+        <f>D63-E63</f>
+        <v>0</v>
+      </c>
+      <c r="I63" s="6">
+        <f>H63/D63*100</f>
+        <v>0</v>
+      </c>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
@@ -4029,15 +4140,33 @@
       <c r="Z63" s="5"/>
     </row>
     <row r="64" ht="13.75" customHeight="1">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
+      <c r="A64" t="s" s="10">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="C64" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="D64" s="5">
+        <v>1</v>
+      </c>
+      <c r="E64" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="F64" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G64" s="5"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
+      <c r="H64" s="6">
+        <f>D64-E64</f>
+        <v>0.2</v>
+      </c>
+      <c r="I64" s="6">
+        <f>H64/D64*100</f>
+        <v>20</v>
+      </c>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
@@ -4057,15 +4186,31 @@
       <c r="Z64" s="5"/>
     </row>
     <row r="65" ht="13.75" customHeight="1">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+      <c r="A65" t="s" s="10">
+        <v>68</v>
+      </c>
+      <c r="B65" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="C65" t="s" s="10">
+        <v>56</v>
+      </c>
+      <c r="D65" s="5">
+        <v>6</v>
+      </c>
       <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
+      <c r="F65" t="s" s="10">
+        <v>57</v>
+      </c>
       <c r="G65" s="5"/>
-      <c r="H65" s="6"/>
-      <c r="I65" s="6"/>
+      <c r="H65" s="6">
+        <f>D65-E65</f>
+        <v>6</v>
+      </c>
+      <c r="I65" s="6">
+        <f>H65/D65*100</f>
+        <v>100</v>
+      </c>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
@@ -30432,95 +30577,11 @@
       <c r="Y1006" s="5"/>
       <c r="Z1006" s="5"/>
     </row>
-    <row r="1007" ht="13.75" customHeight="1">
-      <c r="A1007" s="5"/>
-      <c r="B1007" s="5"/>
-      <c r="C1007" s="5"/>
-      <c r="D1007" s="5"/>
-      <c r="E1007" s="5"/>
-      <c r="F1007" s="5"/>
-      <c r="G1007" s="5"/>
-      <c r="H1007" s="6"/>
-      <c r="I1007" s="6"/>
-      <c r="J1007" s="5"/>
-      <c r="K1007" s="5"/>
-      <c r="L1007" s="5"/>
-      <c r="M1007" s="5"/>
-      <c r="N1007" s="5"/>
-      <c r="O1007" s="5"/>
-      <c r="P1007" s="5"/>
-      <c r="Q1007" s="5"/>
-      <c r="R1007" s="5"/>
-      <c r="S1007" s="5"/>
-      <c r="T1007" s="5"/>
-      <c r="U1007" s="5"/>
-      <c r="V1007" s="5"/>
-      <c r="W1007" s="5"/>
-      <c r="X1007" s="5"/>
-      <c r="Y1007" s="5"/>
-      <c r="Z1007" s="5"/>
-    </row>
-    <row r="1008" ht="13.75" customHeight="1">
-      <c r="A1008" s="5"/>
-      <c r="B1008" s="5"/>
-      <c r="C1008" s="5"/>
-      <c r="D1008" s="5"/>
-      <c r="E1008" s="5"/>
-      <c r="F1008" s="5"/>
-      <c r="G1008" s="5"/>
-      <c r="H1008" s="6"/>
-      <c r="I1008" s="6"/>
-      <c r="J1008" s="5"/>
-      <c r="K1008" s="5"/>
-      <c r="L1008" s="5"/>
-      <c r="M1008" s="5"/>
-      <c r="N1008" s="5"/>
-      <c r="O1008" s="5"/>
-      <c r="P1008" s="5"/>
-      <c r="Q1008" s="5"/>
-      <c r="R1008" s="5"/>
-      <c r="S1008" s="5"/>
-      <c r="T1008" s="5"/>
-      <c r="U1008" s="5"/>
-      <c r="V1008" s="5"/>
-      <c r="W1008" s="5"/>
-      <c r="X1008" s="5"/>
-      <c r="Y1008" s="5"/>
-      <c r="Z1008" s="5"/>
-    </row>
-    <row r="1009" ht="13.75" customHeight="1">
-      <c r="A1009" s="5"/>
-      <c r="B1009" s="5"/>
-      <c r="C1009" s="5"/>
-      <c r="D1009" s="5"/>
-      <c r="E1009" s="5"/>
-      <c r="F1009" s="5"/>
-      <c r="G1009" s="5"/>
-      <c r="H1009" s="6"/>
-      <c r="I1009" s="6"/>
-      <c r="J1009" s="5"/>
-      <c r="K1009" s="5"/>
-      <c r="L1009" s="5"/>
-      <c r="M1009" s="5"/>
-      <c r="N1009" s="5"/>
-      <c r="O1009" s="5"/>
-      <c r="P1009" s="5"/>
-      <c r="Q1009" s="5"/>
-      <c r="R1009" s="5"/>
-      <c r="S1009" s="5"/>
-      <c r="T1009" s="5"/>
-      <c r="U1009" s="5"/>
-      <c r="V1009" s="5"/>
-      <c r="W1009" s="5"/>
-      <c r="X1009" s="5"/>
-      <c r="Y1009" s="5"/>
-      <c r="Z1009" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Adds Status Tracker as of Week 13
</commit_message>
<xml_diff>
--- a/Documents/StatusTracker.xlsx
+++ b/Documents/StatusTracker.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
   <si>
     <t>PROJECT NUMBER</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Anubhab Sen, Vighnesh Chenthil Kumar, Ananya Trivedi</t>
   </si>
   <si>
-    <t>Ongoing</t>
-  </si>
-  <si>
     <t>Week 8 (Sep 27 - October 3)</t>
   </si>
   <si>
@@ -218,6 +215,15 @@
   </si>
   <si>
     <t>Train the bot with the FAQs for FitMeals</t>
+  </si>
+  <si>
+    <t>Week 13 (November 1 - November 7)</t>
+  </si>
+  <si>
+    <t>Update Test Plan</t>
+  </si>
+  <si>
+    <t>Update Design Document</t>
   </si>
 </sst>
 </file>
@@ -342,7 +348,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -374,6 +380,9 @@
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -3452,18 +3461,20 @@
       <c r="D47" s="5">
         <v>15</v>
       </c>
-      <c r="E47" s="5"/>
+      <c r="E47" s="5">
+        <v>10</v>
+      </c>
       <c r="F47" t="s" s="10">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="G47" s="5"/>
       <c r="H47" s="6">
         <f>D47-E47</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="I47" s="6">
         <f>H47/D47*100</f>
-        <v>100</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
@@ -3485,7 +3496,7 @@
     </row>
     <row r="48" ht="13.75" customHeight="1">
       <c r="A48" t="s" s="7">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
@@ -3653,7 +3664,7 @@
     </row>
     <row r="52" ht="13.75" customHeight="1">
       <c r="A52" t="s" s="10">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s" s="10">
         <v>29</v>
@@ -3699,7 +3710,7 @@
     </row>
     <row r="53" ht="13.75" customHeight="1">
       <c r="A53" t="s" s="10">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" t="s" s="10">
         <v>29</v>
@@ -3745,7 +3756,7 @@
     </row>
     <row r="54" ht="13.75" customHeight="1">
       <c r="A54" t="s" s="10">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s" s="10">
         <v>29</v>
@@ -3791,7 +3802,7 @@
     </row>
     <row r="55" ht="13.75" customHeight="1">
       <c r="A55" t="s" s="7">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -3867,7 +3878,7 @@
     </row>
     <row r="57" ht="13.75" customHeight="1">
       <c r="A57" t="s" s="7">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -3943,7 +3954,7 @@
     </row>
     <row r="59" ht="13.75" customHeight="1">
       <c r="A59" t="s" s="7">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -4019,7 +4030,7 @@
     </row>
     <row r="61" ht="13.75" customHeight="1">
       <c r="A61" t="s" s="10">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s" s="10">
         <v>21</v>
@@ -4065,7 +4076,7 @@
     </row>
     <row r="62" ht="13.75" customHeight="1">
       <c r="A62" t="s" s="7">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -4141,7 +4152,7 @@
     </row>
     <row r="64" ht="13.75" customHeight="1">
       <c r="A64" t="s" s="10">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64" t="s" s="10">
         <v>21</v>
@@ -4187,29 +4198,31 @@
     </row>
     <row r="65" ht="13.75" customHeight="1">
       <c r="A65" t="s" s="10">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s" s="10">
         <v>21</v>
       </c>
       <c r="C65" t="s" s="10">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="D65" s="5">
-        <v>6</v>
-      </c>
-      <c r="E65" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E65" s="5">
+        <v>2</v>
+      </c>
       <c r="F65" t="s" s="10">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="G65" s="5"/>
       <c r="H65" s="6">
         <f>D65-E65</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I65" s="6">
         <f>H65/D65*100</f>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
@@ -4230,13 +4243,15 @@
       <c r="Z65" s="5"/>
     </row>
     <row r="66" ht="13.75" customHeight="1">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
+      <c r="A66" t="s" s="7">
+        <v>68</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
       <c r="J66" s="5"/>
@@ -4258,15 +4273,33 @@
       <c r="Z66" s="5"/>
     </row>
     <row r="67" ht="13.75" customHeight="1">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
+      <c r="A67" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="B67" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C67" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="D67" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E67" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="F67" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G67" s="5"/>
-      <c r="H67" s="6"/>
-      <c r="I67" s="6"/>
+      <c r="H67" s="6">
+        <f>D67-E67</f>
+        <v>0</v>
+      </c>
+      <c r="I67" s="6">
+        <f>H67/D67*100</f>
+        <v>0</v>
+      </c>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
@@ -4286,15 +4319,33 @@
       <c r="Z67" s="5"/>
     </row>
     <row r="68" ht="13.75" customHeight="1">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
+      <c r="A68" t="s" s="10">
+        <v>69</v>
+      </c>
+      <c r="B68" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C68" t="s" s="10">
+        <v>24</v>
+      </c>
+      <c r="D68" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="E68" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F68" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G68" s="5"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
+      <c r="H68" s="6">
+        <f>D68-E68</f>
+        <v>0.25</v>
+      </c>
+      <c r="I68" s="6">
+        <f>H68/D68*100</f>
+        <v>33.33333333333333</v>
+      </c>
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
@@ -4314,15 +4365,33 @@
       <c r="Z68" s="5"/>
     </row>
     <row r="69" ht="13.75" customHeight="1">
-      <c r="A69" s="5"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
+      <c r="A69" t="s" s="10">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="C69" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="D69" s="5">
+        <v>2</v>
+      </c>
+      <c r="E69" s="5">
+        <v>3</v>
+      </c>
+      <c r="F69" t="s" s="10">
+        <v>19</v>
+      </c>
       <c r="G69" s="5"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
+      <c r="H69" s="6">
+        <f>D69-E69</f>
+        <v>-1</v>
+      </c>
+      <c r="I69" s="6">
+        <f>H69/D69*100</f>
+        <v>-50</v>
+      </c>
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
@@ -30579,9 +30648,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>